<commit_message>
Change code added defs
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/george/Documents/Github_R/Regrassion_GDP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA78194-33CA-D34F-83A3-BB0FE249E9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6808EAA7-8929-8741-AC13-88DC28FF2985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="15760" xr2:uid="{3580B857-6E9C-4522-A1C6-485FA67992EC}"/>
   </bookViews>
@@ -543,7 +543,7 @@
   <dimension ref="A1:L366"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -552,13 +552,13 @@
     <col min="2" max="2" width="13.5" style="8" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" style="8" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="8" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="8" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="8" customWidth="1"/>
     <col min="6" max="6" width="16.5" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="8" customWidth="1"/>
     <col min="8" max="8" width="20" style="8" customWidth="1"/>
     <col min="9" max="9" width="16.1640625" style="8" customWidth="1"/>
     <col min="10" max="10" width="16.5" style="8" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="8"/>
+    <col min="11" max="11" width="13.5" style="8" customWidth="1"/>
     <col min="12" max="12" width="8.83203125" style="8" customWidth="1"/>
     <col min="13" max="16384" width="8.83203125" style="8"/>
   </cols>
@@ -577,13 +577,13 @@
         <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>5</v>
@@ -610,14 +610,14 @@
       <c r="D2" s="8">
         <v>2356338.2999999998</v>
       </c>
-      <c r="E2" s="3">
-        <v>83.013333333333335</v>
+      <c r="E2" s="10">
+        <v>83.106999999999999</v>
       </c>
       <c r="F2" s="9">
         <v>47.641474747473332</v>
       </c>
-      <c r="G2" s="10">
-        <v>83.106999999999999</v>
+      <c r="G2" s="3">
+        <v>83.013333333333335</v>
       </c>
       <c r="H2" s="3">
         <v>59.1</v>
@@ -628,7 +628,7 @@
       <c r="J2" s="11">
         <v>-0.73775997003258043</v>
       </c>
-      <c r="K2" s="5"/>
+      <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -644,14 +644,14 @@
       <c r="D3" s="8">
         <v>2380453.2999999998</v>
       </c>
-      <c r="E3" s="3">
-        <v>84.736666666666665</v>
+      <c r="E3" s="10">
+        <v>83.007999999999996</v>
       </c>
       <c r="F3" s="9">
         <v>51.609956709956663</v>
       </c>
-      <c r="G3" s="10">
-        <v>83.007999999999996</v>
+      <c r="G3" s="3">
+        <v>84.736666666666665</v>
       </c>
       <c r="H3" s="3">
         <v>59.8</v>
@@ -662,7 +662,7 @@
       <c r="J3" s="11">
         <v>-0.19198564170647303</v>
       </c>
-      <c r="K3" s="5"/>
+      <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -678,14 +678,14 @@
       <c r="D4" s="8">
         <v>2413478</v>
       </c>
-      <c r="E4" s="3">
-        <v>83.95</v>
+      <c r="E4" s="10">
+        <v>83.248000000000005</v>
       </c>
       <c r="F4" s="9">
         <v>61.550288600290003</v>
       </c>
-      <c r="G4" s="10">
-        <v>83.248000000000005</v>
+      <c r="G4" s="3">
+        <v>83.95</v>
       </c>
       <c r="H4" s="3">
         <v>59.8</v>
@@ -696,7 +696,7 @@
       <c r="J4" s="11">
         <v>1.192834114240922</v>
       </c>
-      <c r="K4" s="5"/>
+      <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -712,14 +712,14 @@
       <c r="D5" s="8">
         <v>2446409.2999999998</v>
       </c>
-      <c r="E5" s="3">
-        <v>85.696666666666658</v>
+      <c r="E5" s="10">
+        <v>83.703000000000003</v>
       </c>
       <c r="F5" s="9">
         <v>56.934801587300001</v>
       </c>
-      <c r="G5" s="10">
-        <v>83.703000000000003</v>
+      <c r="G5" s="3">
+        <v>85.696666666666658</v>
       </c>
       <c r="H5" s="3">
         <v>59.8</v>
@@ -730,7 +730,7 @@
       <c r="J5" s="11">
         <v>-0.91325168755096142</v>
       </c>
-      <c r="K5" s="5"/>
+      <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -746,14 +746,14 @@
       <c r="D6" s="8">
         <v>2481974.7000000002</v>
       </c>
-      <c r="E6" s="3">
-        <v>85.63333333333334</v>
+      <c r="E6" s="10">
+        <v>85.477000000000004</v>
       </c>
       <c r="F6" s="9">
         <v>61.916776397516664</v>
       </c>
-      <c r="G6" s="10">
-        <v>85.477000000000004</v>
+      <c r="G6" s="3">
+        <v>85.63333333333334</v>
       </c>
       <c r="H6" s="3">
         <v>60</v>
@@ -764,7 +764,7 @@
       <c r="J6" s="11">
         <v>1.5590381083053757</v>
       </c>
-      <c r="K6" s="5"/>
+      <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -780,14 +780,14 @@
       <c r="D7" s="8">
         <v>2525498.4</v>
       </c>
-      <c r="E7" s="3">
-        <v>87.64</v>
+      <c r="E7" s="10">
+        <v>87.918000000000006</v>
       </c>
       <c r="F7" s="9">
         <v>69.829035087720001</v>
       </c>
-      <c r="G7" s="10">
-        <v>87.918000000000006</v>
+      <c r="G7" s="3">
+        <v>87.64</v>
       </c>
       <c r="H7" s="3">
         <v>60.6</v>
@@ -798,7 +798,7 @@
       <c r="J7" s="11">
         <v>-0.5887718042761283</v>
       </c>
-      <c r="K7" s="5"/>
+      <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -814,14 +814,14 @@
       <c r="D8" s="8">
         <v>2556118.1</v>
       </c>
-      <c r="E8" s="3">
-        <v>86.88666666666667</v>
+      <c r="E8" s="10">
+        <v>89.328000000000003</v>
       </c>
       <c r="F8" s="9">
         <v>70.093740510693337</v>
       </c>
-      <c r="G8" s="10">
-        <v>89.328000000000003</v>
+      <c r="G8" s="3">
+        <v>86.88666666666667</v>
       </c>
       <c r="H8" s="3">
         <v>61.1</v>
@@ -832,7 +832,7 @@
       <c r="J8" s="11">
         <v>-0.78878743245589156</v>
       </c>
-      <c r="K8" s="5"/>
+      <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
     <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -848,14 +848,14 @@
       <c r="D9" s="8">
         <v>2603872.1</v>
       </c>
-      <c r="E9" s="3">
-        <v>88.416666666666671</v>
+      <c r="E9" s="10">
+        <v>88.421999999999997</v>
       </c>
       <c r="F9" s="9">
         <v>59.725972886763337</v>
       </c>
-      <c r="G9" s="10">
-        <v>88.421999999999997</v>
+      <c r="G9" s="3">
+        <v>88.416666666666671</v>
       </c>
       <c r="H9" s="3">
         <v>60.5</v>
@@ -866,7 +866,7 @@
       <c r="J9" s="11">
         <v>0.68505926437646025</v>
       </c>
-      <c r="K9" s="5"/>
+      <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -882,14 +882,14 @@
       <c r="D10" s="8">
         <v>2649569.4</v>
       </c>
-      <c r="E10" s="3">
-        <v>88.153333333333322</v>
+      <c r="E10" s="10">
+        <v>92.24</v>
       </c>
       <c r="F10" s="9">
         <v>58.066575757576665</v>
       </c>
-      <c r="G10" s="10">
-        <v>92.24</v>
+      <c r="G10" s="3">
+        <v>88.153333333333322</v>
       </c>
       <c r="H10" s="3">
         <v>60.2</v>
@@ -900,7 +900,7 @@
       <c r="J10" s="11">
         <v>-1.9501731862862451E-4</v>
       </c>
-      <c r="K10" s="5"/>
+      <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -916,14 +916,14 @@
       <c r="D11" s="8">
         <v>2682738.1</v>
       </c>
-      <c r="E11" s="3">
-        <v>89.923333333333332</v>
+      <c r="E11" s="10">
+        <v>92.816000000000003</v>
       </c>
       <c r="F11" s="9">
         <v>68.730232828446674</v>
       </c>
-      <c r="G11" s="10">
-        <v>92.816000000000003</v>
+      <c r="G11" s="3">
+        <v>89.923333333333332</v>
       </c>
       <c r="H11" s="3">
         <v>61</v>
@@ -934,7 +934,7 @@
       <c r="J11" s="11">
         <v>0.71383169521439682</v>
       </c>
-      <c r="K11" s="5"/>
+      <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -950,14 +950,14 @@
       <c r="D12" s="8">
         <v>2710938.8</v>
       </c>
-      <c r="E12" s="3">
-        <v>89.326666666666668</v>
+      <c r="E12" s="10">
+        <v>95.6</v>
       </c>
       <c r="F12" s="9">
         <v>75.042537549406674</v>
       </c>
-      <c r="G12" s="10">
-        <v>95.6</v>
+      <c r="G12" s="3">
+        <v>89.326666666666668</v>
       </c>
       <c r="H12" s="3">
         <v>61.3</v>
@@ -968,7 +968,7 @@
       <c r="J12" s="11">
         <v>-0.30034869756010396</v>
       </c>
-      <c r="K12" s="5"/>
+      <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -984,14 +984,14 @@
       <c r="D13" s="8">
         <v>2751016.7</v>
       </c>
-      <c r="E13" s="3">
-        <v>91.59333333333332</v>
+      <c r="E13" s="10">
+        <v>102.46299999999999</v>
       </c>
       <c r="F13" s="9">
         <v>88.945335968379993</v>
       </c>
-      <c r="G13" s="10">
-        <v>102.46299999999999</v>
+      <c r="G13" s="3">
+        <v>91.59333333333332</v>
       </c>
       <c r="H13" s="3">
         <v>61</v>
@@ -1002,7 +1002,7 @@
       <c r="J13" s="11">
         <v>-7.30294149308479E-2</v>
       </c>
-      <c r="K13" s="5"/>
+      <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1018,14 +1018,14 @@
       <c r="D14" s="8">
         <v>2785158.7</v>
       </c>
-      <c r="E14" s="3">
-        <v>91.926666666666662</v>
+      <c r="E14" s="10">
+        <v>102.688</v>
       </c>
       <c r="F14" s="9">
         <v>96.671540404040002</v>
       </c>
-      <c r="G14" s="10">
-        <v>102.688</v>
+      <c r="G14" s="3">
+        <v>91.926666666666662</v>
       </c>
       <c r="H14" s="3">
         <v>60.8</v>
@@ -1036,7 +1036,7 @@
       <c r="J14" s="11">
         <v>-1.4042505984193532</v>
       </c>
-      <c r="K14" s="5"/>
+      <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1052,14 +1052,14 @@
       <c r="D15" s="8">
         <v>2801520</v>
       </c>
-      <c r="E15" s="3">
-        <v>94.21</v>
+      <c r="E15" s="10">
+        <v>103.261</v>
       </c>
       <c r="F15" s="9">
         <v>122.39082972582999</v>
       </c>
-      <c r="G15" s="10">
-        <v>103.261</v>
+      <c r="G15" s="3">
+        <v>94.21</v>
       </c>
       <c r="H15" s="3">
         <v>61.8</v>
@@ -1070,7 +1070,7 @@
       <c r="J15" s="11">
         <v>1.7213579177417264</v>
       </c>
-      <c r="K15" s="5"/>
+      <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1086,14 +1086,14 @@
       <c r="D16" s="8">
         <v>2803978.5</v>
       </c>
-      <c r="E16" s="3">
-        <v>93.64</v>
+      <c r="E16" s="10">
+        <v>100.626</v>
       </c>
       <c r="F16" s="9">
         <v>115.59539400213333</v>
       </c>
-      <c r="G16" s="10">
-        <v>100.626</v>
+      <c r="G16" s="3">
+        <v>93.64</v>
       </c>
       <c r="H16" s="3">
         <v>61.8</v>
@@ -1104,7 +1104,7 @@
       <c r="J16" s="11">
         <v>-1.5767515739417697</v>
       </c>
-      <c r="K16" s="5"/>
+      <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1120,14 +1120,14 @@
       <c r="D17" s="8">
         <v>2742042.2</v>
       </c>
-      <c r="E17" s="3">
-        <v>94.40666666666668</v>
+      <c r="E17" s="10">
+        <v>93.873000000000005</v>
       </c>
       <c r="F17" s="9">
         <v>55.888172595519997</v>
       </c>
-      <c r="G17" s="10">
-        <v>93.873000000000005</v>
+      <c r="G17" s="3">
+        <v>94.40666666666668</v>
       </c>
       <c r="H17" s="3">
         <v>61.3</v>
@@ -1138,7 +1138,7 @@
       <c r="J17" s="11">
         <v>-1.7583398755939481</v>
       </c>
-      <c r="K17" s="5"/>
+      <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1154,14 +1154,14 @@
       <c r="D18" s="8">
         <v>2641341.2999999998</v>
       </c>
-      <c r="E18" s="3">
-        <v>93.56</v>
+      <c r="E18" s="10">
+        <v>86.546000000000006</v>
       </c>
       <c r="F18" s="9">
         <v>44.980530303030001</v>
       </c>
-      <c r="G18" s="10">
-        <v>86.546000000000006</v>
+      <c r="G18" s="3">
+        <v>93.56</v>
       </c>
       <c r="H18" s="3">
         <v>60.6</v>
@@ -1172,7 +1172,7 @@
       <c r="J18" s="11">
         <v>-1.0256399232721072</v>
       </c>
-      <c r="K18" s="5"/>
+      <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1188,14 +1188,14 @@
       <c r="D19" s="8">
         <v>2646829.7999999998</v>
       </c>
-      <c r="E19" s="3">
-        <v>95.006666666666675</v>
+      <c r="E19" s="10">
+        <v>82.778000000000006</v>
       </c>
       <c r="F19" s="9">
         <v>59.13433621933666</v>
       </c>
-      <c r="G19" s="10">
-        <v>82.778000000000006</v>
+      <c r="G19" s="3">
+        <v>95.006666666666675</v>
       </c>
       <c r="H19" s="3">
         <v>61.2</v>
@@ -1206,7 +1206,7 @@
       <c r="J19" s="11">
         <v>-0.51116077137761884</v>
       </c>
-      <c r="K19" s="5"/>
+      <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1222,14 +1222,14 @@
       <c r="D20" s="8">
         <v>2669703.2000000002</v>
       </c>
-      <c r="E20" s="3">
-        <v>94.396666666666661</v>
+      <c r="E20" s="10">
+        <v>82.094999999999999</v>
       </c>
       <c r="F20" s="9">
         <v>68.367193362193333</v>
       </c>
-      <c r="G20" s="10">
-        <v>82.094999999999999</v>
+      <c r="G20" s="3">
+        <v>94.396666666666661</v>
       </c>
       <c r="H20" s="3">
         <v>61.3</v>
@@ -1240,7 +1240,7 @@
       <c r="J20" s="11">
         <v>8.6249471352584983E-2</v>
       </c>
-      <c r="K20" s="5"/>
+      <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1256,14 +1256,14 @@
       <c r="D21" s="8">
         <v>2692020.8</v>
       </c>
-      <c r="E21" s="3">
-        <v>96.26</v>
+      <c r="E21" s="10">
+        <v>79.882000000000005</v>
       </c>
       <c r="F21" s="9">
         <v>74.966767676770004</v>
       </c>
-      <c r="G21" s="10">
-        <v>79.882000000000005</v>
+      <c r="G21" s="3">
+        <v>96.26</v>
       </c>
       <c r="H21" s="3">
         <v>60.3</v>
@@ -1274,7 +1274,7 @@
       <c r="J21" s="11">
         <v>-0.79358764095720524</v>
       </c>
-      <c r="K21" s="5"/>
+      <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1290,14 +1290,14 @@
       <c r="D22" s="8">
         <v>2712271.4</v>
       </c>
-      <c r="E22" s="3">
-        <v>96.40666666666668</v>
+      <c r="E22" s="10">
+        <v>84.873000000000005</v>
       </c>
       <c r="F22" s="9">
         <v>76.653260869566665</v>
       </c>
-      <c r="G22" s="10">
-        <v>84.873000000000005</v>
+      <c r="G22" s="3">
+        <v>96.40666666666668</v>
       </c>
       <c r="H22" s="3">
         <v>59.6</v>
@@ -1308,7 +1308,7 @@
       <c r="J22" s="11">
         <v>-0.59686859583268548</v>
       </c>
-      <c r="K22" s="5"/>
+      <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1324,14 +1324,14 @@
       <c r="D23" s="8">
         <v>2747893.6</v>
       </c>
-      <c r="E23" s="3">
-        <v>99.836666666666659</v>
+      <c r="E23" s="10">
+        <v>86.335999999999999</v>
       </c>
       <c r="F23" s="9">
         <v>78.689235209233331</v>
       </c>
-      <c r="G23" s="10">
-        <v>86.335999999999999</v>
+      <c r="G23" s="3">
+        <v>99.836666666666659</v>
       </c>
       <c r="H23" s="3">
         <v>59.7</v>
@@ -1342,7 +1342,7 @@
       <c r="J23" s="11">
         <v>-0.55406273382459503</v>
       </c>
-      <c r="K23" s="5"/>
+      <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
     <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1358,14 +1358,14 @@
       <c r="D24" s="8">
         <v>2775611.3</v>
       </c>
-      <c r="E24" s="3">
-        <v>99.686666666666667</v>
+      <c r="E24" s="10">
+        <v>84.918000000000006</v>
       </c>
       <c r="F24" s="9">
         <v>76.405151515149996</v>
       </c>
-      <c r="G24" s="10">
-        <v>84.918000000000006</v>
+      <c r="G24" s="3">
+        <v>99.686666666666667</v>
       </c>
       <c r="H24" s="3">
         <v>59.3</v>
@@ -1376,7 +1376,7 @@
       <c r="J24" s="11">
         <v>-1.9931790907010718</v>
       </c>
-      <c r="K24" s="5"/>
+      <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
     <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1392,14 +1392,14 @@
       <c r="D25" s="8">
         <v>2801450.8</v>
       </c>
-      <c r="E25" s="3">
-        <v>101.13333333333333</v>
+      <c r="E25" s="10">
+        <v>90.337999999999994</v>
       </c>
       <c r="F25" s="9">
         <v>86.794872325743327</v>
       </c>
-      <c r="G25" s="10">
-        <v>90.337999999999994</v>
+      <c r="G25" s="3">
+        <v>101.13333333333333</v>
       </c>
       <c r="H25" s="3">
         <v>57.8</v>
@@ -1410,7 +1410,7 @@
       <c r="J25" s="11">
         <v>1.9196749896078236</v>
       </c>
-      <c r="K25" s="5"/>
+      <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
     <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1426,14 +1426,14 @@
       <c r="D26" s="8">
         <v>2845988.5</v>
       </c>
-      <c r="E26" s="3">
-        <v>100.7</v>
+      <c r="E26" s="10">
+        <v>86.296000000000006</v>
       </c>
       <c r="F26" s="9">
         <v>104.89703002070667</v>
       </c>
-      <c r="G26" s="10">
-        <v>86.296000000000006</v>
+      <c r="G26" s="3">
+        <v>100.7</v>
       </c>
       <c r="H26" s="3">
         <v>56.4</v>
@@ -1444,7 +1444,7 @@
       <c r="J26" s="11">
         <v>-1.0393872832222939</v>
       </c>
-      <c r="K26" s="5"/>
+      <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
     <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1460,14 +1460,14 @@
       <c r="D27" s="8">
         <v>2852764.2</v>
       </c>
-      <c r="E27" s="3">
-        <v>103.13333333333333</v>
+      <c r="E27" s="10">
+        <v>87.831000000000003</v>
       </c>
       <c r="F27" s="9">
         <v>117.09530303030333</v>
       </c>
-      <c r="G27" s="10">
-        <v>87.831000000000003</v>
+      <c r="G27" s="3">
+        <v>103.13333333333333</v>
       </c>
       <c r="H27" s="3">
         <v>56</v>
@@ -1478,7 +1478,7 @@
       <c r="J27" s="11">
         <v>-2.1873605828584051</v>
       </c>
-      <c r="K27" s="5"/>
+      <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
     <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1494,14 +1494,14 @@
       <c r="D28" s="8">
         <v>2856616.2</v>
       </c>
-      <c r="E28" s="3">
-        <v>101.82333333333334</v>
+      <c r="E28" s="10">
+        <v>89.034000000000006</v>
       </c>
       <c r="F28" s="9">
         <v>112.47346508563999</v>
       </c>
-      <c r="G28" s="10">
-        <v>89.034000000000006</v>
+      <c r="G28" s="3">
+        <v>101.82333333333334</v>
       </c>
       <c r="H28" s="3">
         <v>55</v>
@@ -1512,7 +1512,7 @@
       <c r="J28" s="11">
         <v>2.5747365793093602</v>
       </c>
-      <c r="K28" s="5"/>
+      <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
     <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1528,14 +1528,14 @@
       <c r="D29" s="8">
         <v>2847827.2</v>
       </c>
-      <c r="E29" s="3">
-        <v>103.78666666666668</v>
+      <c r="E29" s="10">
+        <v>85.216999999999999</v>
       </c>
       <c r="F29" s="9">
         <v>109.29390331890333</v>
       </c>
-      <c r="G29" s="10">
-        <v>85.216999999999999</v>
+      <c r="G29" s="3">
+        <v>103.78666666666668</v>
       </c>
       <c r="H29" s="3">
         <v>53</v>
@@ -1546,7 +1546,7 @@
       <c r="J29" s="11">
         <v>-3.3202200547679723</v>
       </c>
-      <c r="K29" s="5"/>
+      <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
     <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1562,14 +1562,14 @@
       <c r="D30" s="8">
         <v>2860406.7</v>
       </c>
-      <c r="E30" s="3">
-        <v>102.40333333333332</v>
+      <c r="E30" s="10">
+        <v>89.397000000000006</v>
       </c>
       <c r="F30" s="9">
         <v>118.59573593073667</v>
       </c>
-      <c r="G30" s="10">
-        <v>89.397000000000006</v>
+      <c r="G30" s="3">
+        <v>102.40333333333332</v>
       </c>
       <c r="H30" s="3">
         <v>51.8</v>
@@ -1580,7 +1580,7 @@
       <c r="J30" s="11">
         <v>0.62476610594101489</v>
       </c>
-      <c r="K30" s="5"/>
+      <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
     <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1596,14 +1596,14 @@
       <c r="D31" s="8">
         <v>2859998.6</v>
       </c>
-      <c r="E31" s="3">
-        <v>104.30666666666667</v>
+      <c r="E31" s="10">
+        <v>87.048000000000002</v>
       </c>
       <c r="F31" s="9">
         <v>108.85809558316333</v>
       </c>
-      <c r="G31" s="10">
-        <v>87.048000000000002</v>
+      <c r="G31" s="3">
+        <v>104.30666666666667</v>
       </c>
       <c r="H31" s="3">
         <v>51.2</v>
@@ -1614,7 +1614,7 @@
       <c r="J31" s="11">
         <v>0.41650335041408948</v>
       </c>
-      <c r="K31" s="5"/>
+      <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
     <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1630,14 +1630,14 @@
       <c r="D32" s="8">
         <v>2877730.6</v>
       </c>
-      <c r="E32" s="3">
-        <v>102.61000000000001</v>
+      <c r="E32" s="10">
+        <v>86.858999999999995</v>
       </c>
       <c r="F32" s="9">
         <v>109.95446969697001</v>
       </c>
-      <c r="G32" s="10">
-        <v>86.858999999999995</v>
+      <c r="G32" s="3">
+        <v>102.61000000000001</v>
       </c>
       <c r="H32" s="3">
         <v>50.5</v>
@@ -1648,7 +1648,7 @@
       <c r="J32" s="11">
         <v>0.24976440085827833</v>
       </c>
-      <c r="K32" s="5"/>
+      <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
     <row r="33" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1664,14 +1664,14 @@
       <c r="D33" s="8">
         <v>2870431.6</v>
       </c>
-      <c r="E33" s="3">
-        <v>104.36</v>
+      <c r="E33" s="10">
+        <v>92.179000000000002</v>
       </c>
       <c r="F33" s="9">
         <v>110.45393214756332</v>
       </c>
-      <c r="G33" s="10">
-        <v>92.179000000000002</v>
+      <c r="G33" s="3">
+        <v>104.36</v>
       </c>
       <c r="H33" s="3">
         <v>49.7</v>
@@ -1682,7 +1682,7 @@
       <c r="J33" s="11">
         <v>-0.98969811056696155</v>
       </c>
-      <c r="K33" s="5"/>
+      <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
     <row r="34" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1698,14 +1698,14 @@
       <c r="D34" s="8">
         <v>2874772.3</v>
       </c>
-      <c r="E34" s="3">
-        <v>102.38333333333333</v>
+      <c r="E34" s="10">
+        <v>87.918999999999997</v>
       </c>
       <c r="F34" s="9">
         <v>112.91104545454665</v>
       </c>
-      <c r="G34" s="10">
-        <v>87.918999999999997</v>
+      <c r="G34" s="3">
+        <v>102.38333333333333</v>
       </c>
       <c r="H34" s="3">
         <v>48.6</v>
@@ -1716,7 +1716,7 @@
       <c r="J34" s="11">
         <v>0.24668328248765481</v>
       </c>
-      <c r="K34" s="5"/>
+      <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
     <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1732,14 +1732,14 @@
       <c r="D35" s="8">
         <v>2897891.5</v>
       </c>
-      <c r="E35" s="3">
-        <v>103.91333333333334</v>
+      <c r="E35" s="10">
+        <v>91.265000000000001</v>
       </c>
       <c r="F35" s="9">
         <v>103.0041370224</v>
       </c>
-      <c r="G35" s="10">
-        <v>91.265000000000001</v>
+      <c r="G35" s="3">
+        <v>103.91333333333334</v>
       </c>
       <c r="H35" s="3">
         <v>49.1</v>
@@ -1750,7 +1750,7 @@
       <c r="J35" s="11">
         <v>1.2587967883962254</v>
       </c>
-      <c r="K35" s="5"/>
+      <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
     <row r="36" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1766,14 +1766,14 @@
       <c r="D36" s="8">
         <v>2909070.5</v>
       </c>
-      <c r="E36" s="3">
-        <v>101.77333333333333</v>
+      <c r="E36" s="10">
+        <v>92.62</v>
       </c>
       <c r="F36" s="9">
         <v>110.10068699416667</v>
       </c>
-      <c r="G36" s="10">
-        <v>92.62</v>
+      <c r="G36" s="3">
+        <v>101.77333333333333</v>
       </c>
       <c r="H36" s="3">
         <v>49.1</v>
@@ -1784,7 +1784,7 @@
       <c r="J36" s="11">
         <v>-1.2104658509298976</v>
       </c>
-      <c r="K36" s="5"/>
+      <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
     <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1800,14 +1800,14 @@
       <c r="D37" s="8">
         <v>2920612.4</v>
       </c>
-      <c r="E37" s="3">
-        <v>102.07666666666667</v>
+      <c r="E37" s="10">
+        <v>89.918000000000006</v>
       </c>
       <c r="F37" s="9">
         <v>109.40962870945334</v>
       </c>
-      <c r="G37" s="10">
-        <v>89.918000000000006</v>
+      <c r="G37" s="3">
+        <v>102.07666666666667</v>
       </c>
       <c r="H37" s="3">
         <v>48.4</v>
@@ -1818,7 +1818,7 @@
       <c r="J37" s="11">
         <v>-0.50056797532180175</v>
       </c>
-      <c r="K37" s="5"/>
+      <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
     <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1834,14 +1834,14 @@
       <c r="D38" s="8">
         <v>2944262.1</v>
       </c>
-      <c r="E38" s="3">
-        <v>101.09999999999998</v>
+      <c r="E38" s="10">
+        <v>95.441000000000003</v>
       </c>
       <c r="F38" s="9">
         <v>107.87666666666667</v>
       </c>
-      <c r="G38" s="10">
-        <v>95.441000000000003</v>
+      <c r="G38" s="3">
+        <v>101.09999999999998</v>
       </c>
       <c r="H38" s="3">
         <v>48.5</v>
@@ -1852,7 +1852,7 @@
       <c r="J38" s="11">
         <v>-0.67816118993914376</v>
       </c>
-      <c r="K38" s="5"/>
+      <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
     <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1868,14 +1868,14 @@
       <c r="D39" s="8">
         <v>2958342.3</v>
       </c>
-      <c r="E39" s="3">
-        <v>102.11666666666666</v>
+      <c r="E39" s="10">
+        <v>95.846000000000004</v>
       </c>
       <c r="F39" s="9">
         <v>109.78000000000002</v>
       </c>
-      <c r="G39" s="10">
-        <v>95.846000000000004</v>
+      <c r="G39" s="3">
+        <v>102.11666666666666</v>
       </c>
       <c r="H39" s="3">
         <v>49.4</v>
@@ -1886,7 +1886,7 @@
       <c r="J39" s="11">
         <v>0.9621542429257971</v>
       </c>
-      <c r="K39" s="5"/>
+      <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
     <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1902,14 +1902,14 @@
       <c r="D40" s="8">
         <v>2978310.5</v>
       </c>
-      <c r="E40" s="3">
-        <v>101.03000000000002</v>
+      <c r="E40" s="10">
+        <v>99.094999999999999</v>
       </c>
       <c r="F40" s="9">
         <v>102.08</v>
       </c>
-      <c r="G40" s="10">
-        <v>99.094999999999999</v>
+      <c r="G40" s="3">
+        <v>101.03000000000002</v>
       </c>
       <c r="H40" s="3">
         <v>50.2</v>
@@ -1920,7 +1920,7 @@
       <c r="J40" s="11">
         <v>-0.96772549278445263</v>
       </c>
-      <c r="K40" s="5"/>
+      <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
     <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1936,14 +1936,14 @@
       <c r="D41" s="8">
         <v>2996687.2</v>
       </c>
-      <c r="E41" s="3">
-        <v>100.18333333333334</v>
+      <c r="E41" s="10">
+        <v>101.28700000000001</v>
       </c>
       <c r="F41" s="9">
         <v>76.013333333333321</v>
       </c>
-      <c r="G41" s="10">
-        <v>101.28700000000001</v>
+      <c r="G41" s="3">
+        <v>100.18333333333334</v>
       </c>
       <c r="H41" s="3">
         <v>49.6</v>
@@ -1954,7 +1954,7 @@
       <c r="J41" s="11">
         <v>-0.10296935563392833</v>
       </c>
-      <c r="K41" s="5"/>
+      <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
     <row r="42" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1970,14 +1970,14 @@
       <c r="D42" s="8">
         <v>3036344.9</v>
       </c>
-      <c r="E42" s="3">
-        <v>98.899999999999991</v>
+      <c r="E42" s="10">
+        <v>102.715</v>
       </c>
       <c r="F42" s="9">
         <v>53.93</v>
       </c>
-      <c r="G42" s="10">
-        <v>102.715</v>
+      <c r="G42" s="3">
+        <v>98.899999999999991</v>
       </c>
       <c r="H42" s="3">
         <v>49.2</v>
@@ -1988,7 +1988,7 @@
       <c r="J42" s="11">
         <v>1.5751187447695123</v>
       </c>
-      <c r="K42" s="5"/>
+      <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
     <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2004,14 +2004,14 @@
       <c r="D43" s="8">
         <v>3068451.1</v>
       </c>
-      <c r="E43" s="3">
-        <v>100.64333333333333</v>
+      <c r="E43" s="10">
+        <v>104.089</v>
       </c>
       <c r="F43" s="9">
         <v>62.096666666666671</v>
       </c>
-      <c r="G43" s="10">
-        <v>104.089</v>
+      <c r="G43" s="3">
+        <v>100.64333333333333</v>
       </c>
       <c r="H43" s="3">
         <v>51</v>
@@ -2022,7 +2022,7 @@
       <c r="J43" s="11">
         <v>-2.3724202990103191</v>
       </c>
-      <c r="K43" s="5"/>
+      <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
     <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2038,14 +2038,14 @@
       <c r="D44" s="8">
         <v>3089545.1</v>
       </c>
-      <c r="E44" s="3">
-        <v>100.21666666666665</v>
+      <c r="E44" s="10">
+        <v>102.009</v>
       </c>
       <c r="F44" s="9">
         <v>50.033333333333331</v>
       </c>
-      <c r="G44" s="10">
-        <v>102.009</v>
+      <c r="G44" s="3">
+        <v>100.21666666666665</v>
       </c>
       <c r="H44" s="3">
         <v>51.7</v>
@@ -2056,7 +2056,7 @@
       <c r="J44" s="11">
         <v>2.0914598473117594</v>
       </c>
-      <c r="K44" s="5"/>
+      <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
     <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2072,14 +2072,14 @@
       <c r="D45" s="8">
         <v>3112248.7</v>
       </c>
-      <c r="E45" s="3">
-        <v>100.24666666666667</v>
+      <c r="E45" s="10">
+        <v>103.35599999999999</v>
       </c>
       <c r="F45" s="9">
         <v>43.419999999999995</v>
       </c>
-      <c r="G45" s="10">
-        <v>103.35599999999999</v>
+      <c r="G45" s="3">
+        <v>100.24666666666667</v>
       </c>
       <c r="H45" s="3">
         <v>51.3</v>
@@ -2090,7 +2090,7 @@
       <c r="J45" s="11">
         <v>1.6850308185153224</v>
       </c>
-      <c r="K45" s="5"/>
+      <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
     <row r="46" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2106,14 +2106,14 @@
       <c r="D46" s="8">
         <v>3128145</v>
       </c>
-      <c r="E46" s="3">
-        <v>98.660000000000011</v>
+      <c r="E46" s="10">
+        <v>100.992</v>
       </c>
       <c r="F46" s="9">
         <v>34.356666666666662</v>
       </c>
-      <c r="G46" s="10">
-        <v>100.992</v>
+      <c r="G46" s="3">
+        <v>98.660000000000011</v>
       </c>
       <c r="H46" s="3">
         <v>50.9</v>
@@ -2124,7 +2124,7 @@
       <c r="J46" s="11">
         <v>-1.9271816030589932</v>
       </c>
-      <c r="K46" s="5"/>
+      <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
     <row r="47" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2140,14 +2140,14 @@
       <c r="D47" s="8">
         <v>3143587</v>
       </c>
-      <c r="E47" s="3">
-        <v>100.50999999999999</v>
+      <c r="E47" s="10">
+        <v>100.64100000000001</v>
       </c>
       <c r="F47" s="9">
         <v>45.953333333333326</v>
       </c>
-      <c r="G47" s="10">
-        <v>100.64100000000001</v>
+      <c r="G47" s="3">
+        <v>100.50999999999999</v>
       </c>
       <c r="H47" s="3">
         <v>52.4</v>
@@ -2158,7 +2158,7 @@
       <c r="J47" s="11">
         <v>0.57964013981868967</v>
       </c>
-      <c r="K47" s="5"/>
+      <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
     <row r="48" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2174,14 +2174,14 @@
       <c r="D48" s="8">
         <v>3166325.6</v>
       </c>
-      <c r="E48" s="3">
-        <v>100.40666666666668</v>
+      <c r="E48" s="10">
+        <v>103.97</v>
       </c>
       <c r="F48" s="9">
         <v>45.800000000000004</v>
       </c>
-      <c r="G48" s="10">
-        <v>103.97</v>
+      <c r="G48" s="3">
+        <v>100.40666666666668</v>
       </c>
       <c r="H48" s="3">
         <v>53</v>
@@ -2192,7 +2192,7 @@
       <c r="J48" s="11">
         <v>0.1760543507322424</v>
       </c>
-      <c r="K48" s="5"/>
+      <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
     <row r="49" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2208,14 +2208,14 @@
       <c r="D49" s="8">
         <v>3193172.7</v>
       </c>
-      <c r="E49" s="3">
-        <v>100.48333333333333</v>
+      <c r="E49" s="10">
+        <v>104.937</v>
       </c>
       <c r="F49" s="9">
         <v>50.079999999999991</v>
       </c>
-      <c r="G49" s="10">
-        <v>104.937</v>
+      <c r="G49" s="3">
+        <v>100.48333333333333</v>
       </c>
       <c r="H49" s="3">
         <v>51.8</v>
@@ -2226,7 +2226,7 @@
       <c r="J49" s="11">
         <v>1.5373846031140133</v>
       </c>
-      <c r="K49" s="5"/>
+      <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
     <row r="50" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2242,14 +2242,14 @@
       <c r="D50" s="8">
         <v>3239565.5</v>
       </c>
-      <c r="E50" s="3">
-        <v>100.18</v>
+      <c r="E50" s="10">
+        <v>107.983</v>
       </c>
       <c r="F50" s="9">
         <v>54.116666666666667</v>
       </c>
-      <c r="G50" s="10">
-        <v>107.983</v>
+      <c r="G50" s="3">
+        <v>100.18</v>
       </c>
       <c r="H50" s="3">
         <v>52</v>
@@ -2260,7 +2260,7 @@
       <c r="J50" s="11">
         <v>0.30629366398365238</v>
       </c>
-      <c r="K50" s="5"/>
+      <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
     <row r="51" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2276,14 +2276,14 @@
       <c r="D51" s="8">
         <v>3277629</v>
       </c>
-      <c r="E51" s="3">
-        <v>101.86</v>
+      <c r="E51" s="10">
+        <v>110.803</v>
       </c>
       <c r="F51" s="9">
         <v>50.24666666666667</v>
       </c>
-      <c r="G51" s="10">
-        <v>110.803</v>
+      <c r="G51" s="3">
+        <v>101.86</v>
       </c>
       <c r="H51" s="3">
         <v>54</v>
@@ -2294,7 +2294,7 @@
       <c r="J51" s="11">
         <v>-0.42316367996083309</v>
       </c>
-      <c r="K51" s="5"/>
+      <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
     <row r="52" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2310,14 +2310,14 @@
       <c r="D52" s="8">
         <v>3312174.1</v>
       </c>
-      <c r="E52" s="3">
-        <v>101.25999999999999</v>
+      <c r="E52" s="10">
+        <v>112.95099999999999</v>
       </c>
       <c r="F52" s="9">
         <v>51.74</v>
       </c>
-      <c r="G52" s="10">
-        <v>112.95099999999999</v>
+      <c r="G52" s="3">
+        <v>101.25999999999999</v>
       </c>
       <c r="H52" s="3">
         <v>54.6</v>
@@ -2328,7 +2328,7 @@
       <c r="J52" s="11">
         <v>-0.50885672719622521</v>
       </c>
-      <c r="K52" s="5"/>
+      <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
     <row r="53" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2344,14 +2344,14 @@
       <c r="D53" s="8">
         <v>3350217.3</v>
       </c>
-      <c r="E53" s="3">
-        <v>101.31333333333333</v>
+      <c r="E53" s="10">
+        <v>113.31</v>
       </c>
       <c r="F53" s="9">
         <v>61.466666666666661</v>
       </c>
-      <c r="G53" s="10">
-        <v>113.31</v>
+      <c r="G53" s="3">
+        <v>101.31333333333333</v>
       </c>
       <c r="H53" s="3">
         <v>53.4</v>
@@ -2362,7 +2362,7 @@
       <c r="J53" s="11">
         <v>1.0639205677284982</v>
       </c>
-      <c r="K53" s="5"/>
+      <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
     <row r="54" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2378,14 +2378,14 @@
       <c r="D54" s="8">
         <v>3371166.9</v>
       </c>
-      <c r="E54" s="3">
-        <v>100.45</v>
+      <c r="E54" s="10">
+        <v>118.01900000000001</v>
       </c>
       <c r="F54" s="9">
         <v>66.953333333333333</v>
       </c>
-      <c r="G54" s="10">
-        <v>118.01900000000001</v>
+      <c r="G54" s="3">
+        <v>100.45</v>
       </c>
       <c r="H54" s="3">
         <v>53.3</v>
@@ -2396,7 +2396,7 @@
       <c r="J54" s="11">
         <v>0.30674607977813068</v>
       </c>
-      <c r="K54" s="5"/>
+      <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
     <row r="55" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2412,14 +2412,14 @@
       <c r="D55" s="8">
         <v>3393630.3</v>
       </c>
-      <c r="E55" s="3">
-        <v>102.61666666666667</v>
+      <c r="E55" s="10">
+        <v>120.474</v>
       </c>
       <c r="F55" s="9">
         <v>74.489999999999995</v>
       </c>
-      <c r="G55" s="10">
-        <v>120.474</v>
+      <c r="G55" s="3">
+        <v>102.61666666666667</v>
       </c>
       <c r="H55" s="3">
         <v>55.3</v>
@@ -2430,7 +2430,7 @@
       <c r="J55" s="11">
         <v>-0.27954881580700253</v>
       </c>
-      <c r="K55" s="5"/>
+      <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
     <row r="56" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2446,14 +2446,14 @@
       <c r="D56" s="8">
         <v>3416540.8</v>
       </c>
-      <c r="E56" s="3">
-        <v>102.20333333333333</v>
+      <c r="E56" s="10">
+        <v>120.706</v>
       </c>
       <c r="F56" s="9">
         <v>75.476666666666674</v>
       </c>
-      <c r="G56" s="10">
-        <v>120.706</v>
+      <c r="G56" s="3">
+        <v>102.20333333333333</v>
       </c>
       <c r="H56" s="3">
         <v>55.9</v>
@@ -2464,7 +2464,7 @@
       <c r="J56" s="11">
         <v>3.9480641484302359E-2</v>
       </c>
-      <c r="K56" s="5"/>
+      <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
     <row r="57" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2480,14 +2480,14 @@
       <c r="D57" s="8">
         <v>3455028.9</v>
       </c>
-      <c r="E57" s="3">
-        <v>102.47666666666667</v>
+      <c r="E57" s="10">
+        <v>126.943</v>
       </c>
       <c r="F57" s="9">
         <v>67.36666666666666</v>
       </c>
-      <c r="G57" s="10">
-        <v>126.943</v>
+      <c r="G57" s="3">
+        <v>102.47666666666667</v>
       </c>
       <c r="H57" s="3">
         <v>55.1</v>
@@ -2498,7 +2498,7 @@
       <c r="J57" s="11">
         <v>0.64013421619929634</v>
       </c>
-      <c r="K57" s="5"/>
+      <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
     <row r="58" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2514,14 +2514,14 @@
       <c r="D58" s="8">
         <v>3493941.2</v>
       </c>
-      <c r="E58" s="3">
-        <v>101.24000000000001</v>
+      <c r="E58" s="10">
+        <v>124.684</v>
       </c>
       <c r="F58" s="9">
         <v>63.27</v>
       </c>
-      <c r="G58" s="10">
-        <v>124.684</v>
+      <c r="G58" s="3">
+        <v>101.24000000000001</v>
       </c>
       <c r="H58" s="3">
         <v>55</v>
@@ -2532,7 +2532,7 @@
       <c r="J58" s="11">
         <v>-0.69750224246385439</v>
       </c>
-      <c r="K58" s="5"/>
+      <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
     <row r="59" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2548,14 +2548,14 @@
       <c r="D59" s="8">
         <v>3522938.2</v>
       </c>
-      <c r="E59" s="3">
-        <v>103.26666666666667</v>
+      <c r="E59" s="10">
+        <v>133.90600000000001</v>
       </c>
       <c r="F59" s="9">
         <v>68.343333333333348</v>
       </c>
-      <c r="G59" s="10">
-        <v>133.90600000000001</v>
+      <c r="G59" s="3">
+        <v>103.26666666666667</v>
       </c>
       <c r="H59" s="3">
         <v>57.1</v>
@@ -2566,7 +2566,7 @@
       <c r="J59" s="11">
         <v>-2.7585673499091634E-2</v>
       </c>
-      <c r="K59" s="5"/>
+      <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
     <row r="60" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2582,14 +2582,14 @@
       <c r="D60" s="8">
         <v>3545913.4</v>
       </c>
-      <c r="E60" s="3">
-        <v>102.45333333333333</v>
+      <c r="E60" s="10">
+        <v>133.57499999999999</v>
       </c>
       <c r="F60" s="9">
         <v>61.859999999999992</v>
       </c>
-      <c r="G60" s="10">
-        <v>133.57499999999999</v>
+      <c r="G60" s="3">
+        <v>102.45333333333333</v>
       </c>
       <c r="H60" s="3">
         <v>57.4</v>
@@ -2600,7 +2600,7 @@
       <c r="J60" s="11">
         <v>0.68063648022636725</v>
       </c>
-      <c r="K60" s="5"/>
+      <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
     <row r="61" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2616,14 +2616,14 @@
       <c r="D61" s="8">
         <v>3570054.1</v>
       </c>
-      <c r="E61" s="3">
-        <v>102.89666666666666</v>
+      <c r="E61" s="10">
+        <v>117.506</v>
       </c>
       <c r="F61" s="9">
         <v>62.653333333333329</v>
       </c>
-      <c r="G61" s="10">
-        <v>117.506</v>
+      <c r="G61" s="3">
+        <v>102.89666666666666</v>
       </c>
       <c r="H61" s="3">
         <v>56.5</v>
@@ -2634,7 +2634,7 @@
       <c r="J61" s="11">
         <v>-1.107800617501322</v>
       </c>
-      <c r="K61" s="5"/>
+      <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
     <row r="62" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2650,14 +2650,14 @@
       <c r="D62" s="8">
         <v>3483352</v>
       </c>
-      <c r="E62" s="3">
-        <v>101.80333333333333</v>
+      <c r="E62" s="10">
+        <v>111.827</v>
       </c>
       <c r="F62" s="9">
         <v>50.526666666666664</v>
       </c>
-      <c r="G62" s="10">
-        <v>111.827</v>
+      <c r="G62" s="3">
+        <v>101.80333333333333</v>
       </c>
       <c r="H62" s="3">
         <v>55.9</v>
@@ -2668,7 +2668,7 @@
       <c r="J62" s="11">
         <v>0.64152818235095455</v>
       </c>
-      <c r="K62" s="5"/>
+      <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
     <row r="63" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2684,14 +2684,14 @@
       <c r="D63" s="8">
         <v>3134250.5</v>
       </c>
-      <c r="E63" s="3">
-        <v>102.06</v>
+      <c r="E63" s="10">
+        <v>95.454999999999998</v>
       </c>
       <c r="F63" s="9">
         <v>31.429999999999996</v>
       </c>
-      <c r="G63" s="10">
-        <v>95.454999999999998</v>
+      <c r="G63" s="3">
+        <v>102.06</v>
       </c>
       <c r="H63" s="3">
         <v>55.8</v>
@@ -2702,7 +2702,7 @@
       <c r="J63" s="11">
         <v>-1.4821295654638504</v>
       </c>
-      <c r="K63" s="5"/>
+      <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
     <row r="64" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2718,14 +2718,14 @@
       <c r="D64" s="8">
         <v>3453617.6</v>
       </c>
-      <c r="E64" s="3">
-        <v>100.17666666666666</v>
+      <c r="E64" s="10">
+        <v>90.138999999999996</v>
       </c>
       <c r="F64" s="9">
         <v>42.72</v>
       </c>
-      <c r="G64" s="10">
-        <v>90.138999999999996</v>
+      <c r="G64" s="3">
+        <v>100.17666666666666</v>
       </c>
       <c r="H64" s="3">
         <v>57</v>
@@ -2736,7 +2736,7 @@
       <c r="J64" s="11">
         <v>1.5398031967424692</v>
       </c>
-      <c r="K64" s="5"/>
+      <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
     <row r="65" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2752,14 +2752,14 @@
       <c r="D65" s="8">
         <v>3499125.7</v>
       </c>
-      <c r="E65" s="3">
-        <v>100.64333333333333</v>
+      <c r="E65" s="10">
+        <v>102.57899999999999</v>
       </c>
       <c r="F65" s="9">
         <v>44.523333333333333</v>
       </c>
-      <c r="G65" s="10">
-        <v>102.57899999999999</v>
+      <c r="G65" s="3">
+        <v>100.64333333333333</v>
       </c>
       <c r="H65" s="3">
         <v>56.4</v>
@@ -2770,7 +2770,7 @@
       <c r="J65" s="11">
         <v>0.97034966989242211</v>
       </c>
-      <c r="K65" s="5"/>
+      <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
     <row r="66" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2786,14 +2786,14 @@
       <c r="D66" s="8">
         <v>3553019.2</v>
       </c>
-      <c r="E66" s="3">
-        <v>99.673333333333332</v>
+      <c r="E66" s="10">
+        <v>110.863</v>
       </c>
       <c r="F66" s="9">
         <v>60.566666666666663</v>
       </c>
-      <c r="G66" s="10">
-        <v>110.863</v>
+      <c r="G66" s="3">
+        <v>99.673333333333332</v>
       </c>
       <c r="H66" s="3">
         <v>52.7</v>
@@ -2804,7 +2804,7 @@
       <c r="J66" s="11">
         <v>1.1374495216736578</v>
       </c>
-      <c r="K66" s="5"/>
+      <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
     <row r="67" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2820,14 +2820,14 @@
       <c r="D67" s="8">
         <v>3643059.4</v>
       </c>
-      <c r="E67" s="3">
-        <v>101.48</v>
+      <c r="E67" s="10">
+        <v>119.20099999999999</v>
       </c>
       <c r="F67" s="9">
         <v>68.626666666666665</v>
       </c>
-      <c r="G67" s="10">
-        <v>119.20099999999999</v>
+      <c r="G67" s="3">
+        <v>101.48</v>
       </c>
       <c r="H67" s="3">
         <v>57</v>
@@ -2838,7 +2838,7 @@
       <c r="J67" s="11">
         <v>-0.49023335149984459</v>
       </c>
-      <c r="K67" s="5"/>
+      <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
     <row r="68" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2854,14 +2854,14 @@
       <c r="D68" s="8">
         <v>3749750.4</v>
       </c>
-      <c r="E68" s="3">
-        <v>101.44666666666666</v>
+      <c r="E68" s="10">
+        <v>134.036</v>
       </c>
       <c r="F68" s="9">
         <v>73.00333333333333</v>
       </c>
-      <c r="G68" s="10">
-        <v>134.036</v>
+      <c r="G68" s="3">
+        <v>101.44666666666666</v>
       </c>
       <c r="H68" s="3">
         <v>60.1</v>
@@ -2872,7 +2872,7 @@
       <c r="J68" s="11">
         <v>2.1347653778548996</v>
       </c>
-      <c r="K68" s="5"/>
+      <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
     <row r="69" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2888,14 +2888,14 @@
       <c r="D69" s="8">
         <v>3829372.7</v>
       </c>
-      <c r="E69" s="3">
-        <v>104.40666666666668</v>
+      <c r="E69" s="10">
+        <v>133.387</v>
       </c>
       <c r="F69" s="9">
         <v>79.576666666666668</v>
       </c>
-      <c r="G69" s="10">
-        <v>133.387</v>
+      <c r="G69" s="3">
+        <v>104.40666666666668</v>
       </c>
       <c r="H69" s="3">
         <v>59.2</v>
@@ -2906,7 +2906,7 @@
       <c r="J69" s="11">
         <v>0.27812451788017778</v>
       </c>
-      <c r="K69" s="5"/>
+      <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
     <row r="70" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2922,14 +2922,14 @@
       <c r="D70" s="8">
         <v>3921454.8</v>
       </c>
-      <c r="E70" s="3">
-        <v>106.23666666666668</v>
+      <c r="E70" s="10">
+        <v>128.58199999999999</v>
       </c>
       <c r="F70" s="9">
         <v>98.96</v>
       </c>
-      <c r="G70" s="10">
-        <v>128.58199999999999</v>
+      <c r="G70" s="3">
+        <v>106.23666666666668</v>
       </c>
       <c r="H70" s="3">
         <v>59.2</v>
@@ -2940,7 +2940,7 @@
       <c r="J70" s="11">
         <v>1.2030928391142157</v>
       </c>
-      <c r="K70" s="5"/>
+      <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
     <row r="71" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2956,14 +2956,14 @@
       <c r="D71" s="8">
         <v>4009713.5</v>
       </c>
-      <c r="E71" s="3">
-        <v>112.06333333333333</v>
+      <c r="E71" s="10">
+        <v>136.18100000000001</v>
       </c>
       <c r="F71" s="9">
         <v>112.74333333333334</v>
       </c>
-      <c r="G71" s="10">
-        <v>136.18100000000001</v>
+      <c r="G71" s="3">
+        <v>112.06333333333333</v>
       </c>
       <c r="H71" s="3">
         <v>61.1</v>
@@ -2974,7 +2974,7 @@
       <c r="J71" s="11">
         <v>-0.40456738939497372</v>
       </c>
-      <c r="K71" s="5"/>
+      <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
     <row r="72" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2990,14 +2990,14 @@
       <c r="D72" s="8">
         <v>4078045.1</v>
       </c>
-      <c r="E72" s="3">
-        <v>113.15333333333335</v>
+      <c r="E72" s="10">
+        <v>132.99100000000001</v>
       </c>
       <c r="F72" s="9">
         <v>99.226666666666645</v>
       </c>
-      <c r="G72" s="10">
-        <v>132.99100000000001</v>
+      <c r="G72" s="3">
+        <v>113.15333333333335</v>
       </c>
       <c r="H72" s="3">
         <v>61.9</v>
@@ -3008,7 +3008,7 @@
       <c r="J72" s="11">
         <v>-1.1023044527198622</v>
       </c>
-      <c r="K72" s="5"/>
+      <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
     <row r="73" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3024,14 +3024,14 @@
       <c r="D73" s="8">
         <v>4151186.2</v>
       </c>
-      <c r="E73" s="3">
-        <v>113.40333333333332</v>
+      <c r="E73" s="10">
+        <v>132.602</v>
       </c>
       <c r="F73" s="9">
         <v>88.366666666666674</v>
       </c>
-      <c r="G73" s="10">
-        <v>132.602</v>
+      <c r="G73" s="3">
+        <v>113.40333333333332</v>
       </c>
       <c r="H73" s="3">
         <v>60.7</v>
@@ -3042,7 +3042,7 @@
       <c r="J73" s="11">
         <v>0.17583495838569732</v>
       </c>
-      <c r="K73" s="5"/>
+      <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
     <row r="74" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3058,14 +3058,14 @@
       <c r="D74" s="8">
         <v>4243632.8</v>
       </c>
-      <c r="E74" s="3">
-        <v>113.02666666666669</v>
+      <c r="E74" s="10">
+        <v>139.52600000000001</v>
       </c>
       <c r="F74" s="9">
         <v>81.443333333333342</v>
       </c>
-      <c r="G74" s="10">
-        <v>139.52600000000001</v>
+      <c r="G74" s="3">
+        <v>113.02666666666669</v>
       </c>
       <c r="H74" s="3">
         <v>60.3</v>
@@ -3076,7 +3076,7 @@
       <c r="J74" s="11">
         <v>1.6714875206993502</v>
       </c>
-      <c r="K74" s="5"/>
+      <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
     <row r="75" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3092,14 +3092,14 @@
       <c r="D75" s="8">
         <v>4302131.5999999996</v>
       </c>
-      <c r="E75" s="3">
-        <v>116.31666666666666</v>
+      <c r="E75" s="10">
+        <v>133.61199999999999</v>
       </c>
       <c r="F75" s="9">
         <v>78.233333333333334</v>
       </c>
-      <c r="G75" s="10">
-        <v>133.61199999999999</v>
+      <c r="G75" s="3">
+        <v>116.31666666666666</v>
       </c>
       <c r="H75" s="3">
         <v>62.4</v>
@@ -3110,7 +3110,7 @@
       <c r="J75" s="11">
         <v>-1.6976220186845974</v>
       </c>
-      <c r="K75" s="5"/>
+      <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
     <row r="76" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3126,14 +3126,14 @@
       <c r="D76" s="8">
         <v>4331508.4000000004</v>
       </c>
-      <c r="E76" s="3">
-        <v>116.66333333333334</v>
+      <c r="E76" s="10">
+        <v>133.23599999999999</v>
       </c>
       <c r="F76" s="9">
         <v>86.754333333333321</v>
       </c>
-      <c r="G76" s="10">
-        <v>133.23599999999999</v>
+      <c r="G76" s="3">
+        <v>116.66333333333334</v>
       </c>
       <c r="H76" s="3">
         <v>62.8</v>
@@ -3144,7 +3144,7 @@
       <c r="J76" s="11">
         <v>0.70474906178332197</v>
       </c>
-      <c r="K76" s="5"/>
+      <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
     <row r="77" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3160,14 +3160,14 @@
       <c r="D77" s="8">
         <v>4387256.3</v>
       </c>
-      <c r="E77" s="3">
-        <v>117.33333333333333</v>
+      <c r="E77" s="10">
+        <v>133.886</v>
       </c>
       <c r="F77" s="9">
         <v>84.034000000000006</v>
       </c>
-      <c r="G77" s="10">
-        <v>133.886</v>
+      <c r="G77" s="3">
+        <v>117.33333333333333</v>
       </c>
       <c r="H77" s="3">
         <v>61.7</v>
@@ -3178,7 +3178,7 @@
       <c r="J77" s="11">
         <v>0.82125937853980469</v>
       </c>
-      <c r="K77" s="5"/>
+      <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
     <row r="78" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3194,14 +3194,14 @@
       <c r="D78" s="8">
         <v>4437765.2</v>
       </c>
-      <c r="E78" s="3">
-        <v>116.68666666666667</v>
+      <c r="E78" s="10">
+        <v>133.86799999999999</v>
       </c>
       <c r="F78" s="9">
         <v>83.146000000000001</v>
       </c>
-      <c r="G78" s="10">
-        <v>133.86799999999999</v>
+      <c r="G78" s="3">
+        <v>116.68666666666667</v>
       </c>
       <c r="H78" s="3">
         <v>61.6</v>
@@ -3212,7 +3212,7 @@
       <c r="J78" s="11">
         <v>0.26336048363269887</v>
       </c>
-      <c r="K78" s="5"/>
+      <c r="K78" s="3"/>
       <c r="L78" s="3"/>
     </row>
     <row r="79" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3228,14 +3228,14 @@
       <c r="D79" s="8">
         <v>4475351.2</v>
       </c>
-      <c r="E79" s="3">
-        <v>119.41666666666667</v>
+      <c r="E79" s="10">
+        <v>136.52199999999999</v>
       </c>
       <c r="F79" s="9">
         <v>84.868000000000009</v>
       </c>
-      <c r="G79" s="10">
-        <v>136.52199999999999</v>
+      <c r="G79" s="3">
+        <v>119.41666666666667</v>
       </c>
       <c r="H79" s="3">
         <v>64</v>
@@ -3246,7 +3246,7 @@
       <c r="J79" s="11">
         <v>1.6587442380861579</v>
       </c>
-      <c r="K79" s="5"/>
+      <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
     <row r="80" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3262,14 +3262,14 @@
       <c r="D80" s="8">
         <v>4523628.8</v>
       </c>
-      <c r="E80" s="3">
-        <v>120.27666666666666</v>
+      <c r="E80" s="10">
+        <v>137.27000000000001</v>
       </c>
       <c r="F80" s="9">
         <v>80.150666666666666</v>
       </c>
-      <c r="G80" s="10">
-        <v>137.27000000000001</v>
+      <c r="G80" s="3">
+        <v>120.27666666666666</v>
       </c>
       <c r="H80" s="3">
         <v>64.099999999999994</v>
@@ -3280,7 +3280,7 @@
       <c r="J80" s="11">
         <v>-1.6037763032745165</v>
       </c>
-      <c r="K80" s="5"/>
+      <c r="K80" s="3"/>
       <c r="L80" s="3"/>
     </row>
     <row r="81" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3296,14 +3296,14 @@
       <c r="D81" s="8">
         <v>4579059.7</v>
       </c>
-      <c r="E81" s="3">
-        <v>120.84666666666668</v>
+      <c r="E81" s="10">
+        <v>138.155</v>
       </c>
       <c r="F81" s="9">
         <v>74.63000000000001</v>
       </c>
-      <c r="G81" s="10">
-        <v>138.155</v>
+      <c r="G81" s="3">
+        <v>120.84666666666668</v>
       </c>
       <c r="H81" s="3">
         <v>63.4</v>
@@ -3314,7 +3314,7 @@
       <c r="J81" s="11">
         <v>1.7833595099956827</v>
       </c>
-      <c r="K81" s="5"/>
+      <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
     <row r="82" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3330,14 +3330,14 @@
       <c r="D82" s="8">
         <v>4631838.2</v>
       </c>
-      <c r="E82" s="3">
-        <v>120.30333333333333</v>
+      <c r="E82" s="10">
+        <v>137.303</v>
       </c>
       <c r="F82" s="9">
         <v>75.645666666666671</v>
       </c>
-      <c r="G82" s="10">
-        <v>137.303</v>
+      <c r="G82" s="3">
+        <v>120.30333333333333</v>
       </c>
       <c r="H82" s="3">
         <v>62.8</v>
@@ -3348,7 +3348,7 @@
       <c r="J82" s="11">
         <v>-1.1536639035252823</v>
       </c>
-      <c r="K82" s="5"/>
+      <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
     <row r="83" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3364,14 +3364,14 @@
       <c r="D83" s="8">
         <v>4672609.5999999996</v>
       </c>
-      <c r="E83" s="3">
-        <v>123.19999999999999</v>
+      <c r="E83" s="10">
+        <v>139.11799999999999</v>
       </c>
       <c r="F83" s="9">
         <v>67.800333333333342</v>
       </c>
-      <c r="G83" s="10">
-        <v>139.11799999999999</v>
+      <c r="G83" s="3">
+        <v>123.19999999999999</v>
       </c>
       <c r="H83" s="3">
         <v>65.3</v>
@@ -3382,7 +3382,7 @@
       <c r="J83" s="11">
         <v>1.2873431486908382</v>
       </c>
-      <c r="K83" s="5"/>
+      <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
     <row r="84" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3395,6 +3395,7 @@
       <c r="G84" s="3"/>
       <c r="H84" s="10"/>
       <c r="J84"/>
+      <c r="K84" s="3"/>
     </row>
     <row r="85" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="6"/>
@@ -3405,6 +3406,7 @@
       <c r="F85" s="9"/>
       <c r="G85" s="3"/>
       <c r="H85" s="10"/>
+      <c r="K85" s="3"/>
     </row>
     <row r="86" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="6"/>
@@ -3415,6 +3417,7 @@
       <c r="F86" s="9"/>
       <c r="G86" s="3"/>
       <c r="H86" s="10"/>
+      <c r="K86" s="3"/>
     </row>
     <row r="87" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="6"/>
@@ -3425,6 +3428,7 @@
       <c r="F87" s="9"/>
       <c r="G87" s="3"/>
       <c r="H87" s="10"/>
+      <c r="K87" s="3"/>
     </row>
     <row r="88" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="6"/>
@@ -3435,6 +3439,7 @@
       <c r="F88" s="9"/>
       <c r="G88" s="3"/>
       <c r="H88" s="10"/>
+      <c r="K88" s="3"/>
     </row>
     <row r="89" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="6"/>
@@ -3445,6 +3450,7 @@
       <c r="F89" s="9"/>
       <c r="G89" s="3"/>
       <c r="H89" s="10"/>
+      <c r="K89" s="3"/>
     </row>
     <row r="90" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="6"/>
@@ -3455,6 +3461,7 @@
       <c r="F90" s="9"/>
       <c r="G90" s="3"/>
       <c r="H90" s="10"/>
+      <c r="K90" s="3"/>
     </row>
     <row r="91" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="6"/>
@@ -3465,6 +3472,7 @@
       <c r="F91" s="9"/>
       <c r="G91" s="3"/>
       <c r="H91" s="10"/>
+      <c r="K91" s="3"/>
     </row>
     <row r="92" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="6"/>
@@ -3475,6 +3483,7 @@
       <c r="F92" s="9"/>
       <c r="G92" s="3"/>
       <c r="H92" s="10"/>
+      <c r="K92" s="3"/>
     </row>
     <row r="93" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="6"/>
@@ -3485,6 +3494,7 @@
       <c r="F93" s="9"/>
       <c r="G93" s="3"/>
       <c r="H93" s="10"/>
+      <c r="K93" s="3"/>
     </row>
     <row r="94" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="6"/>
@@ -3495,6 +3505,7 @@
       <c r="F94" s="9"/>
       <c r="G94" s="3"/>
       <c r="H94" s="10"/>
+      <c r="K94" s="3"/>
     </row>
     <row r="95" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="6"/>
@@ -3505,6 +3516,7 @@
       <c r="F95" s="9"/>
       <c r="G95" s="3"/>
       <c r="H95" s="10"/>
+      <c r="K95" s="3"/>
     </row>
     <row r="96" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="6"/>
@@ -3515,8 +3527,9 @@
       <c r="F96" s="9"/>
       <c r="G96" s="3"/>
       <c r="H96" s="10"/>
-    </row>
-    <row r="97" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K96" s="3"/>
+    </row>
+    <row r="97" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="6"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -3525,8 +3538,9 @@
       <c r="F97" s="9"/>
       <c r="G97" s="3"/>
       <c r="H97" s="10"/>
-    </row>
-    <row r="98" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K97" s="3"/>
+    </row>
+    <row r="98" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="6"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -3535,8 +3549,9 @@
       <c r="F98" s="9"/>
       <c r="G98" s="3"/>
       <c r="H98" s="10"/>
-    </row>
-    <row r="99" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K98" s="3"/>
+    </row>
+    <row r="99" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="6"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -3545,8 +3560,9 @@
       <c r="F99" s="9"/>
       <c r="G99" s="3"/>
       <c r="H99" s="10"/>
-    </row>
-    <row r="100" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K99" s="3"/>
+    </row>
+    <row r="100" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="6"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -3555,8 +3571,9 @@
       <c r="F100" s="9"/>
       <c r="G100" s="3"/>
       <c r="H100" s="10"/>
-    </row>
-    <row r="101" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K100" s="3"/>
+    </row>
+    <row r="101" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="6"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -3565,8 +3582,9 @@
       <c r="F101" s="9"/>
       <c r="G101" s="3"/>
       <c r="H101" s="10"/>
-    </row>
-    <row r="102" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K101" s="3"/>
+    </row>
+    <row r="102" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="6"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -3575,8 +3593,9 @@
       <c r="F102" s="9"/>
       <c r="G102" s="3"/>
       <c r="H102" s="10"/>
-    </row>
-    <row r="103" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K102" s="3"/>
+    </row>
+    <row r="103" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="6"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -3585,8 +3604,9 @@
       <c r="F103" s="9"/>
       <c r="G103" s="3"/>
       <c r="H103" s="10"/>
-    </row>
-    <row r="104" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K103" s="3"/>
+    </row>
+    <row r="104" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="6"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -3595,8 +3615,9 @@
       <c r="F104" s="9"/>
       <c r="G104" s="3"/>
       <c r="H104" s="10"/>
-    </row>
-    <row r="105" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K104" s="3"/>
+    </row>
+    <row r="105" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="6"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -3605,8 +3626,9 @@
       <c r="F105" s="9"/>
       <c r="G105" s="3"/>
       <c r="H105" s="10"/>
-    </row>
-    <row r="106" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K105" s="3"/>
+    </row>
+    <row r="106" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="6"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -3615,8 +3637,9 @@
       <c r="F106" s="9"/>
       <c r="G106" s="3"/>
       <c r="H106" s="10"/>
-    </row>
-    <row r="107" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K106" s="3"/>
+    </row>
+    <row r="107" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="6"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -3625,8 +3648,9 @@
       <c r="F107" s="9"/>
       <c r="G107" s="3"/>
       <c r="H107" s="10"/>
-    </row>
-    <row r="108" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K107" s="3"/>
+    </row>
+    <row r="108" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="6"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -3635,8 +3659,9 @@
       <c r="F108" s="9"/>
       <c r="G108" s="3"/>
       <c r="H108" s="10"/>
-    </row>
-    <row r="109" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K108" s="3"/>
+    </row>
+    <row r="109" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="6"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -3645,8 +3670,9 @@
       <c r="F109" s="9"/>
       <c r="G109" s="3"/>
       <c r="H109" s="10"/>
-    </row>
-    <row r="110" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K109" s="3"/>
+    </row>
+    <row r="110" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="6"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -3655,8 +3681,9 @@
       <c r="F110" s="9"/>
       <c r="G110" s="3"/>
       <c r="H110" s="10"/>
-    </row>
-    <row r="111" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K110" s="3"/>
+    </row>
+    <row r="111" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="6"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -3665,8 +3692,9 @@
       <c r="F111" s="9"/>
       <c r="G111" s="3"/>
       <c r="H111" s="10"/>
-    </row>
-    <row r="112" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K111" s="3"/>
+    </row>
+    <row r="112" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="6"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -3675,8 +3703,9 @@
       <c r="F112" s="9"/>
       <c r="G112" s="3"/>
       <c r="H112" s="10"/>
-    </row>
-    <row r="113" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K112" s="3"/>
+    </row>
+    <row r="113" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="6"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -3685,8 +3714,9 @@
       <c r="F113" s="9"/>
       <c r="G113" s="3"/>
       <c r="H113" s="10"/>
-    </row>
-    <row r="114" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K113" s="3"/>
+    </row>
+    <row r="114" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="6"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -3695,8 +3725,9 @@
       <c r="F114" s="9"/>
       <c r="G114" s="3"/>
       <c r="H114" s="10"/>
-    </row>
-    <row r="115" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K114" s="3"/>
+    </row>
+    <row r="115" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="6"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -3705,8 +3736,9 @@
       <c r="F115" s="9"/>
       <c r="G115" s="3"/>
       <c r="H115" s="10"/>
-    </row>
-    <row r="116" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K115" s="3"/>
+    </row>
+    <row r="116" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="6"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -3715,8 +3747,9 @@
       <c r="F116" s="9"/>
       <c r="G116" s="3"/>
       <c r="H116" s="10"/>
-    </row>
-    <row r="117" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K116" s="3"/>
+    </row>
+    <row r="117" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="6"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -3725,8 +3758,9 @@
       <c r="F117" s="9"/>
       <c r="G117" s="3"/>
       <c r="H117" s="10"/>
-    </row>
-    <row r="118" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K117" s="3"/>
+    </row>
+    <row r="118" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="6"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -3735,8 +3769,9 @@
       <c r="F118" s="9"/>
       <c r="G118" s="3"/>
       <c r="H118" s="10"/>
-    </row>
-    <row r="119" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K118" s="3"/>
+    </row>
+    <row r="119" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="6"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -3745,8 +3780,9 @@
       <c r="F119" s="9"/>
       <c r="G119" s="3"/>
       <c r="H119" s="10"/>
-    </row>
-    <row r="120" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K119" s="3"/>
+    </row>
+    <row r="120" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="6"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -3755,8 +3791,9 @@
       <c r="F120" s="9"/>
       <c r="G120" s="3"/>
       <c r="H120" s="10"/>
-    </row>
-    <row r="121" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K120" s="3"/>
+    </row>
+    <row r="121" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="6"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -3765,8 +3802,9 @@
       <c r="F121" s="9"/>
       <c r="G121" s="3"/>
       <c r="H121" s="10"/>
-    </row>
-    <row r="122" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K121" s="3"/>
+    </row>
+    <row r="122" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="12"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -3774,24 +3812,25 @@
       <c r="E122" s="3"/>
       <c r="F122" s="9"/>
       <c r="G122" s="3"/>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K122" s="3"/>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" s="12"/>
       <c r="B123" s="3"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" s="12"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" s="12"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" s="12"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" s="12"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" s="12"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added dummies, mode models
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/george/Documents/Github_R/Regrassion_GDP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6808EAA7-8929-8741-AC13-88DC28FF2985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7D4DD7-3DCE-744F-847A-0CF5AD72D702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="15760" xr2:uid="{3580B857-6E9C-4522-A1C6-485FA67992EC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>DATE</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>10Y BOND INT</t>
+  </si>
+  <si>
+    <t>Dcovid</t>
+  </si>
+  <si>
+    <t>DGFC</t>
   </si>
 </sst>
 </file>
@@ -181,7 +187,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -218,6 +224,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -543,7 +552,7 @@
   <dimension ref="A1:L366"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -594,8 +603,12 @@
       <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
@@ -628,8 +641,12 @@
       <c r="J2" s="11">
         <v>-0.73775997003258043</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="K2" s="14">
+        <v>0</v>
+      </c>
+      <c r="L2" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
@@ -662,8 +679,12 @@
       <c r="J3" s="11">
         <v>-0.19198564170647303</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="K3" s="14">
+        <v>0</v>
+      </c>
+      <c r="L3" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
@@ -696,8 +717,12 @@
       <c r="J4" s="11">
         <v>1.192834114240922</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="K4" s="14">
+        <v>0</v>
+      </c>
+      <c r="L4" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
@@ -730,8 +755,12 @@
       <c r="J5" s="11">
         <v>-0.91325168755096142</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="K5" s="14">
+        <v>0</v>
+      </c>
+      <c r="L5" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
@@ -764,8 +793,12 @@
       <c r="J6" s="11">
         <v>1.5590381083053757</v>
       </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="K6" s="14">
+        <v>0</v>
+      </c>
+      <c r="L6" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
@@ -798,8 +831,12 @@
       <c r="J7" s="11">
         <v>-0.5887718042761283</v>
       </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="K7" s="14">
+        <v>0</v>
+      </c>
+      <c r="L7" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
@@ -832,8 +869,12 @@
       <c r="J8" s="11">
         <v>-0.78878743245589156</v>
       </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="K8" s="14">
+        <v>0</v>
+      </c>
+      <c r="L8" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
@@ -866,8 +907,12 @@
       <c r="J9" s="11">
         <v>0.68505926437646025</v>
       </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="K9" s="14">
+        <v>0</v>
+      </c>
+      <c r="L9" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
@@ -900,8 +945,12 @@
       <c r="J10" s="11">
         <v>-1.9501731862862451E-4</v>
       </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="K10" s="14">
+        <v>0</v>
+      </c>
+      <c r="L10" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
@@ -934,8 +983,12 @@
       <c r="J11" s="11">
         <v>0.71383169521439682</v>
       </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="K11" s="14">
+        <v>0</v>
+      </c>
+      <c r="L11" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
@@ -968,8 +1021,12 @@
       <c r="J12" s="11">
         <v>-0.30034869756010396</v>
       </c>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="K12" s="14">
+        <v>0</v>
+      </c>
+      <c r="L12" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
@@ -1002,8 +1059,12 @@
       <c r="J13" s="11">
         <v>-7.30294149308479E-2</v>
       </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="K13" s="14">
+        <v>0</v>
+      </c>
+      <c r="L13" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
@@ -1036,8 +1097,12 @@
       <c r="J14" s="11">
         <v>-1.4042505984193532</v>
       </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="K14" s="14">
+        <v>0</v>
+      </c>
+      <c r="L14" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
@@ -1070,8 +1135,12 @@
       <c r="J15" s="11">
         <v>1.7213579177417264</v>
       </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="K15" s="14">
+        <v>0</v>
+      </c>
+      <c r="L15" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
@@ -1104,8 +1173,12 @@
       <c r="J16" s="11">
         <v>-1.5767515739417697</v>
       </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="K16" s="14">
+        <v>0</v>
+      </c>
+      <c r="L16" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
@@ -1138,8 +1211,12 @@
       <c r="J17" s="11">
         <v>-1.7583398755939481</v>
       </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="K17" s="14">
+        <v>0</v>
+      </c>
+      <c r="L17" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
@@ -1172,8 +1249,12 @@
       <c r="J18" s="11">
         <v>-1.0256399232721072</v>
       </c>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="K18" s="14">
+        <v>0</v>
+      </c>
+      <c r="L18" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
@@ -1206,8 +1287,12 @@
       <c r="J19" s="11">
         <v>-0.51116077137761884</v>
       </c>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="K19" s="14">
+        <v>0</v>
+      </c>
+      <c r="L19" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
@@ -1240,8 +1325,12 @@
       <c r="J20" s="11">
         <v>8.6249471352584983E-2</v>
       </c>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="K20" s="14">
+        <v>0</v>
+      </c>
+      <c r="L20" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
@@ -1274,8 +1363,12 @@
       <c r="J21" s="11">
         <v>-0.79358764095720524</v>
       </c>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
+      <c r="K21" s="14">
+        <v>0</v>
+      </c>
+      <c r="L21" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
@@ -1308,8 +1401,12 @@
       <c r="J22" s="11">
         <v>-0.59686859583268548</v>
       </c>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+      <c r="K22" s="14">
+        <v>0</v>
+      </c>
+      <c r="L22" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
@@ -1342,8 +1439,12 @@
       <c r="J23" s="11">
         <v>-0.55406273382459503</v>
       </c>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="K23" s="14">
+        <v>0</v>
+      </c>
+      <c r="L23" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
@@ -1376,8 +1477,12 @@
       <c r="J24" s="11">
         <v>-1.9931790907010718</v>
       </c>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
+      <c r="K24" s="14">
+        <v>0</v>
+      </c>
+      <c r="L24" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
@@ -1410,8 +1515,12 @@
       <c r="J25" s="11">
         <v>1.9196749896078236</v>
       </c>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
+      <c r="K25" s="14">
+        <v>0</v>
+      </c>
+      <c r="L25" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
@@ -1444,8 +1553,12 @@
       <c r="J26" s="11">
         <v>-1.0393872832222939</v>
       </c>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
+      <c r="K26" s="14">
+        <v>0</v>
+      </c>
+      <c r="L26" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
@@ -1478,8 +1591,12 @@
       <c r="J27" s="11">
         <v>-2.1873605828584051</v>
       </c>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
+      <c r="K27" s="14">
+        <v>0</v>
+      </c>
+      <c r="L27" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
@@ -1512,8 +1629,12 @@
       <c r="J28" s="11">
         <v>2.5747365793093602</v>
       </c>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
+      <c r="K28" s="14">
+        <v>0</v>
+      </c>
+      <c r="L28" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
@@ -1546,8 +1667,12 @@
       <c r="J29" s="11">
         <v>-3.3202200547679723</v>
       </c>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
+      <c r="K29" s="14">
+        <v>0</v>
+      </c>
+      <c r="L29" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
@@ -1580,8 +1705,12 @@
       <c r="J30" s="11">
         <v>0.62476610594101489</v>
       </c>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
+      <c r="K30" s="14">
+        <v>0</v>
+      </c>
+      <c r="L30" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
@@ -1614,8 +1743,12 @@
       <c r="J31" s="11">
         <v>0.41650335041408948</v>
       </c>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
+      <c r="K31" s="14">
+        <v>0</v>
+      </c>
+      <c r="L31" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
@@ -1648,8 +1781,12 @@
       <c r="J32" s="11">
         <v>0.24976440085827833</v>
       </c>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
+      <c r="K32" s="14">
+        <v>0</v>
+      </c>
+      <c r="L32" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
@@ -1682,8 +1819,12 @@
       <c r="J33" s="11">
         <v>-0.98969811056696155</v>
       </c>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
+      <c r="K33" s="14">
+        <v>0</v>
+      </c>
+      <c r="L33" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
@@ -1716,8 +1857,12 @@
       <c r="J34" s="11">
         <v>0.24668328248765481</v>
       </c>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
+      <c r="K34" s="14">
+        <v>0</v>
+      </c>
+      <c r="L34" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
@@ -1750,8 +1895,12 @@
       <c r="J35" s="11">
         <v>1.2587967883962254</v>
       </c>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
+      <c r="K35" s="14">
+        <v>0</v>
+      </c>
+      <c r="L35" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
@@ -1784,8 +1933,12 @@
       <c r="J36" s="11">
         <v>-1.2104658509298976</v>
       </c>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
+      <c r="K36" s="14">
+        <v>0</v>
+      </c>
+      <c r="L36" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
@@ -1818,8 +1971,12 @@
       <c r="J37" s="11">
         <v>-0.50056797532180175</v>
       </c>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
+      <c r="K37" s="14">
+        <v>0</v>
+      </c>
+      <c r="L37" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
@@ -1852,8 +2009,12 @@
       <c r="J38" s="11">
         <v>-0.67816118993914376</v>
       </c>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
+      <c r="K38" s="14">
+        <v>0</v>
+      </c>
+      <c r="L38" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
@@ -1886,8 +2047,12 @@
       <c r="J39" s="11">
         <v>0.9621542429257971</v>
       </c>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
+      <c r="K39" s="14">
+        <v>0</v>
+      </c>
+      <c r="L39" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
@@ -1920,8 +2085,12 @@
       <c r="J40" s="11">
         <v>-0.96772549278445263</v>
       </c>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
+      <c r="K40" s="14">
+        <v>0</v>
+      </c>
+      <c r="L40" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
@@ -1954,8 +2123,12 @@
       <c r="J41" s="11">
         <v>-0.10296935563392833</v>
       </c>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
+      <c r="K41" s="14">
+        <v>0</v>
+      </c>
+      <c r="L41" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
@@ -1988,8 +2161,12 @@
       <c r="J42" s="11">
         <v>1.5751187447695123</v>
       </c>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
+      <c r="K42" s="14">
+        <v>0</v>
+      </c>
+      <c r="L42" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
@@ -2022,8 +2199,12 @@
       <c r="J43" s="11">
         <v>-2.3724202990103191</v>
       </c>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
+      <c r="K43" s="14">
+        <v>0</v>
+      </c>
+      <c r="L43" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
@@ -2056,8 +2237,12 @@
       <c r="J44" s="11">
         <v>2.0914598473117594</v>
       </c>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
+      <c r="K44" s="14">
+        <v>0</v>
+      </c>
+      <c r="L44" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
@@ -2090,8 +2275,12 @@
       <c r="J45" s="11">
         <v>1.6850308185153224</v>
       </c>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
+      <c r="K45" s="14">
+        <v>0</v>
+      </c>
+      <c r="L45" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
@@ -2124,8 +2313,12 @@
       <c r="J46" s="11">
         <v>-1.9271816030589932</v>
       </c>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
+      <c r="K46" s="14">
+        <v>0</v>
+      </c>
+      <c r="L46" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
@@ -2158,8 +2351,12 @@
       <c r="J47" s="11">
         <v>0.57964013981868967</v>
       </c>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
+      <c r="K47" s="14">
+        <v>0</v>
+      </c>
+      <c r="L47" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
@@ -2192,8 +2389,12 @@
       <c r="J48" s="11">
         <v>0.1760543507322424</v>
       </c>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
+      <c r="K48" s="14">
+        <v>0</v>
+      </c>
+      <c r="L48" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
@@ -2226,8 +2427,12 @@
       <c r="J49" s="11">
         <v>1.5373846031140133</v>
       </c>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
+      <c r="K49" s="14">
+        <v>0</v>
+      </c>
+      <c r="L49" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
@@ -2260,8 +2465,12 @@
       <c r="J50" s="11">
         <v>0.30629366398365238</v>
       </c>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
+      <c r="K50" s="14">
+        <v>0</v>
+      </c>
+      <c r="L50" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
@@ -2294,8 +2503,12 @@
       <c r="J51" s="11">
         <v>-0.42316367996083309</v>
       </c>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
+      <c r="K51" s="14">
+        <v>0</v>
+      </c>
+      <c r="L51" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
@@ -2328,8 +2541,12 @@
       <c r="J52" s="11">
         <v>-0.50885672719622521</v>
       </c>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
+      <c r="K52" s="14">
+        <v>0</v>
+      </c>
+      <c r="L52" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
@@ -2362,8 +2579,12 @@
       <c r="J53" s="11">
         <v>1.0639205677284982</v>
       </c>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
+      <c r="K53" s="14">
+        <v>0</v>
+      </c>
+      <c r="L53" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
@@ -2396,8 +2617,12 @@
       <c r="J54" s="11">
         <v>0.30674607977813068</v>
       </c>
-      <c r="K54" s="3"/>
-      <c r="L54" s="3"/>
+      <c r="K54" s="14">
+        <v>0</v>
+      </c>
+      <c r="L54" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="6">
@@ -2430,8 +2655,12 @@
       <c r="J55" s="11">
         <v>-0.27954881580700253</v>
       </c>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
+      <c r="K55" s="14">
+        <v>0</v>
+      </c>
+      <c r="L55" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
@@ -2464,8 +2693,12 @@
       <c r="J56" s="11">
         <v>3.9480641484302359E-2</v>
       </c>
-      <c r="K56" s="3"/>
-      <c r="L56" s="3"/>
+      <c r="K56" s="14">
+        <v>0</v>
+      </c>
+      <c r="L56" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
@@ -2498,8 +2731,12 @@
       <c r="J57" s="11">
         <v>0.64013421619929634</v>
       </c>
-      <c r="K57" s="3"/>
-      <c r="L57" s="3"/>
+      <c r="K57" s="14">
+        <v>0</v>
+      </c>
+      <c r="L57" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
@@ -2532,8 +2769,12 @@
       <c r="J58" s="11">
         <v>-0.69750224246385439</v>
       </c>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
+      <c r="K58" s="14">
+        <v>0</v>
+      </c>
+      <c r="L58" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="59" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
@@ -2566,8 +2807,12 @@
       <c r="J59" s="11">
         <v>-2.7585673499091634E-2</v>
       </c>
-      <c r="K59" s="3"/>
-      <c r="L59" s="3"/>
+      <c r="K59" s="14">
+        <v>0</v>
+      </c>
+      <c r="L59" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
@@ -2600,8 +2845,12 @@
       <c r="J60" s="11">
         <v>0.68063648022636725</v>
       </c>
-      <c r="K60" s="3"/>
-      <c r="L60" s="3"/>
+      <c r="K60" s="14">
+        <v>0</v>
+      </c>
+      <c r="L60" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
@@ -2634,8 +2883,12 @@
       <c r="J61" s="11">
         <v>-1.107800617501322</v>
       </c>
-      <c r="K61" s="3"/>
-      <c r="L61" s="3"/>
+      <c r="K61" s="14">
+        <v>0</v>
+      </c>
+      <c r="L61" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
@@ -2668,8 +2921,12 @@
       <c r="J62" s="11">
         <v>0.64152818235095455</v>
       </c>
-      <c r="K62" s="3"/>
-      <c r="L62" s="3"/>
+      <c r="K62" s="14">
+        <v>0</v>
+      </c>
+      <c r="L62" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
@@ -2702,8 +2959,12 @@
       <c r="J63" s="11">
         <v>-1.4821295654638504</v>
       </c>
-      <c r="K63" s="3"/>
-      <c r="L63" s="3"/>
+      <c r="K63" s="14">
+        <v>1</v>
+      </c>
+      <c r="L63" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
@@ -2736,8 +2997,12 @@
       <c r="J64" s="11">
         <v>1.5398031967424692</v>
       </c>
-      <c r="K64" s="3"/>
-      <c r="L64" s="3"/>
+      <c r="K64" s="14">
+        <v>1</v>
+      </c>
+      <c r="L64" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
@@ -2770,8 +3035,12 @@
       <c r="J65" s="11">
         <v>0.97034966989242211</v>
       </c>
-      <c r="K65" s="3"/>
-      <c r="L65" s="3"/>
+      <c r="K65" s="14">
+        <v>1</v>
+      </c>
+      <c r="L65" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="66" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="6">
@@ -2804,8 +3073,12 @@
       <c r="J66" s="11">
         <v>1.1374495216736578</v>
       </c>
-      <c r="K66" s="3"/>
-      <c r="L66" s="3"/>
+      <c r="K66" s="14">
+        <v>1</v>
+      </c>
+      <c r="L66" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="6">
@@ -2838,8 +3111,12 @@
       <c r="J67" s="11">
         <v>-0.49023335149984459</v>
       </c>
-      <c r="K67" s="3"/>
-      <c r="L67" s="3"/>
+      <c r="K67" s="14">
+        <v>1</v>
+      </c>
+      <c r="L67" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="68" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="6">
@@ -2872,8 +3149,12 @@
       <c r="J68" s="11">
         <v>2.1347653778548996</v>
       </c>
-      <c r="K68" s="3"/>
-      <c r="L68" s="3"/>
+      <c r="K68" s="14">
+        <v>1</v>
+      </c>
+      <c r="L68" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="6">
@@ -2906,8 +3187,12 @@
       <c r="J69" s="11">
         <v>0.27812451788017778</v>
       </c>
-      <c r="K69" s="3"/>
-      <c r="L69" s="3"/>
+      <c r="K69" s="14">
+        <v>0</v>
+      </c>
+      <c r="L69" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
@@ -2940,8 +3225,12 @@
       <c r="J70" s="11">
         <v>1.2030928391142157</v>
       </c>
-      <c r="K70" s="3"/>
-      <c r="L70" s="3"/>
+      <c r="K70" s="14">
+        <v>0</v>
+      </c>
+      <c r="L70" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="71" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="6">
@@ -2974,8 +3263,12 @@
       <c r="J71" s="11">
         <v>-0.40456738939497372</v>
       </c>
-      <c r="K71" s="3"/>
-      <c r="L71" s="3"/>
+      <c r="K71" s="14">
+        <v>0</v>
+      </c>
+      <c r="L71" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
@@ -3008,8 +3301,12 @@
       <c r="J72" s="11">
         <v>-1.1023044527198622</v>
       </c>
-      <c r="K72" s="3"/>
-      <c r="L72" s="3"/>
+      <c r="K72" s="14">
+        <v>0</v>
+      </c>
+      <c r="L72" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="6">
@@ -3042,8 +3339,12 @@
       <c r="J73" s="11">
         <v>0.17583495838569732</v>
       </c>
-      <c r="K73" s="3"/>
-      <c r="L73" s="3"/>
+      <c r="K73" s="14">
+        <v>0</v>
+      </c>
+      <c r="L73" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="74" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="6">
@@ -3076,8 +3377,12 @@
       <c r="J74" s="11">
         <v>1.6714875206993502</v>
       </c>
-      <c r="K74" s="3"/>
-      <c r="L74" s="3"/>
+      <c r="K74" s="14">
+        <v>0</v>
+      </c>
+      <c r="L74" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="6">
@@ -3110,8 +3415,12 @@
       <c r="J75" s="11">
         <v>-1.6976220186845974</v>
       </c>
-      <c r="K75" s="3"/>
-      <c r="L75" s="3"/>
+      <c r="K75" s="14">
+        <v>0</v>
+      </c>
+      <c r="L75" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="6">
@@ -3144,8 +3453,12 @@
       <c r="J76" s="11">
         <v>0.70474906178332197</v>
       </c>
-      <c r="K76" s="3"/>
-      <c r="L76" s="3"/>
+      <c r="K76" s="14">
+        <v>0</v>
+      </c>
+      <c r="L76" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="77" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="6">
@@ -3178,8 +3491,12 @@
       <c r="J77" s="11">
         <v>0.82125937853980469</v>
       </c>
-      <c r="K77" s="3"/>
-      <c r="L77" s="3"/>
+      <c r="K77" s="14">
+        <v>0</v>
+      </c>
+      <c r="L77" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="6">
@@ -3212,8 +3529,12 @@
       <c r="J78" s="11">
         <v>0.26336048363269887</v>
       </c>
-      <c r="K78" s="3"/>
-      <c r="L78" s="3"/>
+      <c r="K78" s="14">
+        <v>0</v>
+      </c>
+      <c r="L78" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="6">
@@ -3246,8 +3567,12 @@
       <c r="J79" s="11">
         <v>1.6587442380861579</v>
       </c>
-      <c r="K79" s="3"/>
-      <c r="L79" s="3"/>
+      <c r="K79" s="14">
+        <v>0</v>
+      </c>
+      <c r="L79" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="6">
@@ -3280,8 +3605,12 @@
       <c r="J80" s="11">
         <v>-1.6037763032745165</v>
       </c>
-      <c r="K80" s="3"/>
-      <c r="L80" s="3"/>
+      <c r="K80" s="14">
+        <v>0</v>
+      </c>
+      <c r="L80" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="81" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="6">
@@ -3314,8 +3643,12 @@
       <c r="J81" s="11">
         <v>1.7833595099956827</v>
       </c>
-      <c r="K81" s="3"/>
-      <c r="L81" s="3"/>
+      <c r="K81" s="14">
+        <v>0</v>
+      </c>
+      <c r="L81" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="6">
@@ -3348,8 +3681,12 @@
       <c r="J82" s="11">
         <v>-1.1536639035252823</v>
       </c>
-      <c r="K82" s="3"/>
-      <c r="L82" s="3"/>
+      <c r="K82" s="14">
+        <v>0</v>
+      </c>
+      <c r="L82" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="83" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="6">
@@ -3382,8 +3719,12 @@
       <c r="J83" s="11">
         <v>1.2873431486908382</v>
       </c>
-      <c r="K83" s="3"/>
-      <c r="L83" s="3"/>
+      <c r="K83" s="14">
+        <v>0</v>
+      </c>
+      <c r="L83" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="84" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="6"/>

</xml_diff>